<commit_message>
six: Resolve issues with bulk upload not working
</commit_message>
<xml_diff>
--- a/mock_candidates.xlsx
+++ b/mock_candidates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,11 +461,6 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>createdBy</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
           <t>location</t>
         </is>
       </c>
@@ -473,49 +468,44 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Stacy Ramirez</t>
+          <t>Joshua Black</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>veronicamitchell@example.com</t>
+          <t>mhart@example.com</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Product Manager</t>
+          <t>UI/UX Designer</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Senior</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>On Hold</t>
+          <t>OFFER ACCEPTED</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Lonnie Mitchell</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Royfurt</t>
+          <t>Watsontown</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Mr. Troy Hall</t>
+          <t>Daniel Cunningham</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>gomezjoshua@example.com</t>
+          <t>derekbell@example.net</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -525,34 +515,29 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Offer Accepted</t>
+          <t>OFFER REJECTED</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Dennis Trujillo</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Ericfort</t>
+          <t>Curtisstad</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Carolyn Hickman</t>
+          <t>Tammy David</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>robertsaaron@example.com</t>
+          <t>robinsonsara@example.org</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -562,34 +547,29 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Mid</t>
+          <t>JUNIOR</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Shortlisted</t>
+          <t>SHORTLISTED</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Dakota Ortega</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Glassport</t>
+          <t>North Keithville</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Laura Jackson</t>
+          <t>Lindsey Williams</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>alexandria62@example.com</t>
+          <t>cobbwilliam@example.com</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -599,108 +579,93 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Senior</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>REJECTED</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Andrew Stephens</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Foxshire</t>
+          <t>Milesland</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Curtis Brown</t>
+          <t>Paul Reed</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>jennifermurphy@example.org</t>
+          <t>deborahlucas@example.com</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Full Stack Developer</t>
+          <t>DevOps Engineer</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>On Hold</t>
+          <t>OFFERED</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Joseph Torres</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>South Dean</t>
+          <t>South Johnton</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Katie Allen</t>
+          <t>Jamie Liu</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>jgross@example.org</t>
+          <t>ggallagher@example.org</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Frontend Developer</t>
+          <t>Product Manager</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>SENIOR</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Offer Rejected</t>
+          <t>ON HOLD</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Scott Martin</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Jennaside</t>
+          <t>Sanchezside</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Amy Cruz</t>
+          <t>Nancy Mann</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>uford@example.com</t>
+          <t>ashley35@example.org</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -710,133 +675,113 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Senior</t>
+          <t>SENIOR</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Hired</t>
+          <t>REJECTED</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Jennifer Fowler</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>East Kimberlyside</t>
+          <t>North Brittneyshire</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Rebecca Patel</t>
+          <t>Crystal Kaufman</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>theresaford@example.org</t>
+          <t>sspencer@example.org</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>UI/UX Designer</t>
+          <t>Backend Developer</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Lead</t>
+          <t>LEAD</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Offered</t>
+          <t>REJECTED</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Joe Wilkinson</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>North Mackenzieshire</t>
+          <t>Khanport</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Mark Schultz</t>
+          <t>Amanda Velazquez</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>zimmermanlinda@example.net</t>
+          <t>bethsmith@example.com</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Frontend Developer</t>
+          <t>DevOps Engineer</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Mid</t>
+          <t>LEAD</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Offered</t>
+          <t>OFFER REJECTED</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Jessica Torres</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>South Nicole</t>
+          <t>Johnland</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Christopher Rodriguez</t>
+          <t>Paul Owens</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>robertsdavid@example.net</t>
+          <t>melissachavez@example.net</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Full Stack Developer</t>
+          <t>Backend Developer</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Mid</t>
+          <t>SENIOR</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Offer Accepted</t>
+          <t>REJECTED</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Alice Mclean</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Perryview</t>
+          <t>Zacharyfort</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Unreject candidate should make the candidate status open and progress pending
</commit_message>
<xml_diff>
--- a/mock_candidates.xlsx
+++ b/mock_candidates.xlsx
@@ -468,44 +468,44 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Joshua Black</t>
+          <t>April Duncan</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>mhart@example.com</t>
+          <t>william36@example.com</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>UI/UX Designer</t>
+          <t>Backend Developer</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>SENIOR</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>OFFER ACCEPTED</t>
+          <t>REJECTED</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Watsontown</t>
+          <t>Gilbertburgh</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Daniel Cunningham</t>
+          <t>Kyle Wheeler</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>derekbell@example.net</t>
+          <t>hhouse@example.com</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -515,103 +515,103 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>SENIOR</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>OFFER REJECTED</t>
+          <t>OFFERED</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Curtisstad</t>
+          <t>Ryanstad</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Tammy David</t>
+          <t>Mitchell Thompson</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>robinsonsara@example.org</t>
+          <t>dfaulkner@example.org</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>DevOps Engineer</t>
+          <t>Backend Developer</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>JUNIOR</t>
+          <t>SENIOR</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>SHORTLISTED</t>
+          <t>HIRED</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>North Keithville</t>
+          <t>New Jackieview</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Lindsey Williams</t>
+          <t>Robert Macias</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>cobbwilliam@example.com</t>
+          <t>hernandezjoshua@example.org</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Backend Developer</t>
+          <t>Full Stack Developer</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>JUNIOR</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>REJECTED</t>
+          <t>OFFERED</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Milesland</t>
+          <t>Jenniferfort</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Paul Reed</t>
+          <t>Cynthia Gonzales</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>deborahlucas@example.com</t>
+          <t>bguerrero@example.net</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>DevOps Engineer</t>
+          <t>UI/UX Designer</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>SENIOR</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -621,88 +621,88 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>South Johnton</t>
+          <t>Wellschester</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Jamie Liu</t>
+          <t>Richard Howard</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ggallagher@example.org</t>
+          <t>jenniferfreeman@example.org</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Product Manager</t>
+          <t>DevOps Engineer</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>SENIOR</t>
+          <t>LEAD</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>ON HOLD</t>
+          <t>ON_HOLD</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Sanchezside</t>
+          <t>Michaelbury</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Nancy Mann</t>
+          <t>Kelly Rose</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ashley35@example.org</t>
+          <t>wschultz@example.com</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Frontend Developer</t>
+          <t>Backend Developer</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>SENIOR</t>
+          <t>JUNIOR</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>REJECTED</t>
+          <t>OFFER_ACCEPTED</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>North Brittneyshire</t>
+          <t>Jenniferland</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Crystal Kaufman</t>
+          <t>Alan Simmons</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>sspencer@example.org</t>
+          <t>dean13@example.net</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Backend Developer</t>
+          <t>Product Manager</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -712,76 +712,76 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>REJECTED</t>
+          <t>SHORTLISTED</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Khanport</t>
+          <t>Watkinshaven</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Amanda Velazquez</t>
+          <t>Kimberly Gonzales</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>bethsmith@example.com</t>
+          <t>hparker@example.net</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>DevOps Engineer</t>
+          <t>Full Stack Developer</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>LEAD</t>
+          <t>JUNIOR</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>OFFER REJECTED</t>
+          <t>REJECTED</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Johnland</t>
+          <t>Nicoleville</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Paul Owens</t>
+          <t>Ryan Dean</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>melissachavez@example.net</t>
+          <t>steven07@example.org</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Backend Developer</t>
+          <t>UI/UX Designer</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>SENIOR</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>REJECTED</t>
+          <t>OFFERED</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Zacharyfort</t>
+          <t>Keithshire</t>
         </is>
       </c>
     </row>

</xml_diff>